<commit_message>
Python SecretSanta - final - entregue
Excel: hide das colunas de turma e grupo
notebook python: clear dos outputs
</commit_message>
<xml_diff>
--- a/Python/Projeto/SecretSantaDataSet.xlsx
+++ b/Python/Projeto/SecretSantaDataSet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anafs\ISEG\repo-dsba-ana\2.1-PPL\Project-SecretSanta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anafs\ISEG\DSBA2023-GrupoX\Python\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2A2FD6-01E9-4AA3-908A-02320C9FA87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DEA7B8-B202-4497-9F85-749B1B127EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,9 +232,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,16 +517,16 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>

</xml_diff>